<commit_message>
file column modified for correct input
</commit_message>
<xml_diff>
--- a/Type_A.xlsx
+++ b/Type_A.xlsx
@@ -55,12 +55,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -73,16 +79,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -99,13 +105,13 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -125,6 +131,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -263,13 +270,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -368,10 +369,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -626,13 +627,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -945,10 +940,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1202,7 +1197,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1268,48 +1263,6 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>